<commit_message>
Added changes to excel sheet
</commit_message>
<xml_diff>
--- a/Final Documentation/results.xlsx
+++ b/Final Documentation/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1068,16 +1068,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1530,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K2:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K3:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new testing results.
</commit_message>
<xml_diff>
--- a/Final Documentation/results.xlsx
+++ b/Final Documentation/results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -44,14 +44,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,31 +83,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="3"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -115,28 +106,30 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Automata approximation</a:t>
+              <a:t>Automata approximation - results for testing set</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>4 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$L$3:$L$12</c:f>
@@ -183,7 +176,6 @@
           <c:tx>
             <c:v>6 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$M$3:$M$12</c:f>
@@ -230,7 +222,6 @@
           <c:tx>
             <c:v>10 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$N$3:$N$12</c:f>
@@ -277,7 +268,6 @@
           <c:tx>
             <c:v>15 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$O$3:$O$12</c:f>
@@ -318,24 +308,14 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="254626432"/>
-        <c:axId val="254672256"/>
+        <c:axId val="74787456"/>
+        <c:axId val="74810496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254626432"/>
+        <c:axId val="74787456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -354,25 +334,27 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254672256"/>
+        <c:crossAx val="74810496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254672256"/>
+        <c:axId val="74810496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -392,29 +374,39 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254626432"/>
+        <c:crossAx val="74787456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86340640809443503"/>
+          <c:y val="0.42627401646544133"/>
+          <c:w val="0.1197301854974705"/>
+          <c:h val="0.25737299107347411"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -422,17 +414,8 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -445,28 +428,29 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>20 states automaton approximation</a:t>
+              <a:t>20 states</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>4 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet5!$L$4:$L$13</c:f>
@@ -477,31 +461,31 @@
                   <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.92</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,7 +497,6 @@
           <c:tx>
             <c:v>6 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet5!$M$4:$M$13</c:f>
@@ -521,10 +504,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.88</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.44</c:v>
@@ -533,7 +516,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.85</c:v>
@@ -542,36 +525,164 @@
                   <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.89</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.86</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="374404224"/>
-        <c:axId val="374405760"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="89225472"/>
+        <c:axId val="89605248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374404224"/>
+        <c:axId val="89225472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -590,25 +701,20 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="374405760"/>
+        <c:crossAx val="89605248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374405760"/>
+        <c:axId val="89605248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -628,13 +734,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="374404224"/>
+        <c:crossAx val="89225472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -642,15 +745,12 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -658,36 +758,43 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>30 states</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>30-states automaton</c:v>
+            <c:v>4 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet6!$N$4:$N$13</c:f>
@@ -698,28 +805,28 @@
                   <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.71</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.98</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.92</c:v>
@@ -728,49 +835,253 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="282600576"/>
-        <c:axId val="282602112"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$R$4:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="102951168"/>
+        <c:axId val="102957440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="282600576"/>
+        <c:axId val="102951168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282602112"/>
+        <c:crossAx val="102957440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="282602112"/>
+        <c:axId val="102957440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282600576"/>
+        <c:crossAx val="102951168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -778,15 +1089,12 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -794,36 +1102,51 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>50</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>states</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>50-states automaton</c:v>
+            <c:v>4 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet7!$M$4:$M$13</c:f>
@@ -834,22 +1157,22 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.89</c:v>
@@ -858,55 +1181,260 @@
                   <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.92</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="358873344"/>
-        <c:axId val="358937344"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="89946368"/>
+        <c:axId val="100462592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="358873344"/>
+        <c:axId val="89946368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358937344"/>
+        <c:crossAx val="100462592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358937344"/>
+        <c:axId val="100462592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358873344"/>
+        <c:crossAx val="89946368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -914,15 +1442,12 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -930,36 +1455,43 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="3"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>80 states</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>80-states automaton</c:v>
+            <c:v>4 states</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet8!$N$6:$N$15</c:f>
@@ -967,7 +1499,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.99</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.99</c:v>
@@ -979,19 +1511,19 @@
                   <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.99</c:v>
@@ -1000,49 +1532,253 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="362438656"/>
-        <c:axId val="362440192"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$O$6:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$P$6:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$Q$6:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet8!$R$6:$R$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="60832000"/>
+        <c:axId val="61018112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="362438656"/>
+        <c:axId val="60832000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362440192"/>
+        <c:crossAx val="61018112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362440192"/>
+        <c:axId val="61018112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362438656"/>
+        <c:crossAx val="60832000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1050,11 +1786,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1068,21 +1801,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="1025" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1104,19 +1839,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="20-states automaton" title="20-states automaton aproximation"/>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1138,20 +1873,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Wykres 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1174,19 +1909,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1209,22 +1944,20 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1242,9 +1975,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1282,7 +2015,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1316,7 +2049,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1351,10 +2083,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1527,16 +2258,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="K2:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="11:15">
       <c r="L2" t="s">
         <v>0</v>
       </c>
@@ -1550,7 +2281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="11:15">
       <c r="K3">
         <v>1</v>
       </c>
@@ -1567,7 +2298,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="11:15">
       <c r="K4">
         <v>2</v>
       </c>
@@ -1584,7 +2315,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="5" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="11:15">
       <c r="K5">
         <v>3</v>
       </c>
@@ -1601,7 +2332,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="6" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="11:15">
       <c r="K6">
         <v>4</v>
       </c>
@@ -1618,7 +2349,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="7" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="11:15">
       <c r="K7">
         <v>5</v>
       </c>
@@ -1635,7 +2366,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="11:15">
       <c r="K8">
         <v>6</v>
       </c>
@@ -1652,7 +2383,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="11:15">
       <c r="K9">
         <v>7</v>
       </c>
@@ -1669,7 +2400,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="10" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="11:15">
       <c r="K10">
         <v>8</v>
       </c>
@@ -1686,7 +2417,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="11:15">
       <c r="K11">
         <v>9</v>
       </c>
@@ -1703,7 +2434,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="12" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="11:15">
       <c r="K12">
         <v>10</v>
       </c>
@@ -1720,7 +2451,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="11:15">
       <c r="K13" t="s">
         <v>4</v>
       </c>
@@ -1742,25 +2473,26 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="K3:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="11:16">
       <c r="L3" t="s">
         <v>0</v>
       </c>
@@ -1777,7 +2509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="11:16">
       <c r="K4">
         <v>1</v>
       </c>
@@ -1785,21 +2517,39 @@
         <v>0.66</v>
       </c>
       <c r="M4">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="5" spans="11:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0.93</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="11:16">
       <c r="K5">
         <v>2</v>
       </c>
       <c r="L5">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="6" spans="11:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="11:16">
       <c r="K6">
         <v>3</v>
       </c>
@@ -1809,19 +2559,37 @@
       <c r="M6">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="7" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="11:16">
       <c r="K7">
         <v>4</v>
       </c>
       <c r="L7">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0.96</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="11:16">
       <c r="K8">
         <v>5</v>
       </c>
@@ -1829,32 +2597,59 @@
         <v>0.95</v>
       </c>
       <c r="M8">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="9" spans="11:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="11:16">
       <c r="K9">
         <v>6</v>
       </c>
       <c r="L9">
-        <v>0.94</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="10" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0.96</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="11:16">
       <c r="K10">
         <v>7</v>
       </c>
       <c r="L10">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="11" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="11:16">
       <c r="K11">
         <v>8</v>
       </c>
@@ -1862,58 +2657,98 @@
         <v>0.95</v>
       </c>
       <c r="M11">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="12" spans="11:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0.97</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="11:16">
       <c r="K12">
         <v>9</v>
       </c>
       <c r="L12">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="13" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0.95</v>
+      </c>
+      <c r="P12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="13" spans="11:16">
       <c r="K13">
         <v>10</v>
       </c>
       <c r="L13">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="14" spans="11:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="11:16">
       <c r="L14">
         <f>AVERAGE(L4:L13)</f>
-        <v>0.92000000000000015</v>
+        <v>0.95100000000000018</v>
       </c>
       <c r="M14">
         <f>AVERAGE(M4:M13)</f>
-        <v>0.84699999999999986</v>
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="N14">
+        <f>AVERAGE(N4:N13)</f>
+        <v>0.98999999999999988</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(O4:O13)</f>
+        <v>0.98699999999999988</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(P4:P13)</f>
+        <v>0.99099999999999999</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="M3:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:R3"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="13:18">
       <c r="N3" t="s">
         <v>0</v>
       </c>
@@ -1930,109 +2765,246 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="13:18">
       <c r="M4">
         <v>1</v>
       </c>
       <c r="N4">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="5" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0.83</v>
+      </c>
+      <c r="Q4">
+        <v>0.78</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="13:18">
       <c r="M5">
         <v>2</v>
       </c>
       <c r="N5">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="6" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0.97</v>
+      </c>
+      <c r="P5">
+        <v>0.99</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="13:18">
       <c r="M6">
         <v>3</v>
       </c>
       <c r="N6">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="7" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="13:18">
       <c r="M7">
         <v>4</v>
       </c>
       <c r="N7">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="8" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0.99</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="13:18">
       <c r="M8">
         <v>5</v>
       </c>
       <c r="N8">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="9" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>0.96</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9" spans="13:18">
       <c r="M9">
         <v>6</v>
       </c>
       <c r="N9">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="10" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="13:18">
       <c r="M10">
         <v>7</v>
       </c>
       <c r="N10">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="11" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0.52</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="13:18">
       <c r="M11">
         <v>8</v>
       </c>
       <c r="N11">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="12" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0.98</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="13:18">
       <c r="M12">
         <v>9</v>
       </c>
       <c r="N12">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="13" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0.89</v>
+      </c>
+      <c r="P12">
+        <v>0.99</v>
+      </c>
+      <c r="Q12">
+        <v>0.81</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="13:18">
       <c r="M13">
         <v>10</v>
       </c>
       <c r="N13">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="14" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="13:18">
       <c r="N14">
         <f>AVERAGE(N4:N13)</f>
-        <v>0.86699999999999999</v>
+        <v>0.94100000000000006</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(O4:O13)</f>
+        <v>0.98000000000000009</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(P4:P13)</f>
+        <v>0.98100000000000009</v>
+      </c>
+      <c r="Q14">
+        <f>AVERAGE(Q4:Q13)</f>
+        <v>0.91000000000000014</v>
+      </c>
+      <c r="R14">
+        <f>AVERAGE(R4:R13)</f>
+        <v>0.999</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="L3:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:Q3"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="12:17">
       <c r="M3" t="s">
         <v>0</v>
       </c>
@@ -2049,109 +3021,246 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="12:17">
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0.99</v>
+      </c>
+      <c r="O4">
+        <v>0.84</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="12:17">
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="6" spans="12:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0.99</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="12:17">
       <c r="L6">
         <v>3</v>
       </c>
       <c r="M6">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="7" spans="12:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="12:17">
       <c r="L7">
         <v>4</v>
       </c>
       <c r="M7">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="8" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0.89</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0.99</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="12:17">
       <c r="L8">
         <v>5</v>
       </c>
       <c r="M8">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="9" spans="12:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0.86</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="12:17">
       <c r="L9">
         <v>6</v>
       </c>
       <c r="M9">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="10" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="12:17">
       <c r="L10">
         <v>7</v>
       </c>
       <c r="M10">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="12:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0.85</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="12:17">
       <c r="L11">
         <v>8</v>
       </c>
       <c r="M11">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="12" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>0.99</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="12:17">
       <c r="L12">
         <v>9</v>
       </c>
       <c r="M12">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="13" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="13" spans="12:17">
       <c r="L13">
         <v>10</v>
       </c>
       <c r="M13">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="14" spans="12:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="14" spans="12:17">
       <c r="M14">
         <f>AVERAGE(M4:M13)</f>
-        <v>0.89699999999999991</v>
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="N14">
+        <f>AVERAGE(N4:N13)</f>
+        <v>0.9870000000000001</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(O4:O13)</f>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(P4:P13)</f>
+        <v>0.999</v>
+      </c>
+      <c r="Q14">
+        <f>AVERAGE(Q4:Q13)</f>
+        <v>0.99299999999999999</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="M5:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:R5"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="13:18">
       <c r="N5" t="s">
         <v>0</v>
       </c>
@@ -2168,93 +3277,230 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="13:18">
       <c r="M6">
         <v>1</v>
       </c>
       <c r="N6">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="7" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0.98</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="7" spans="13:18">
       <c r="M7">
         <v>2</v>
       </c>
       <c r="N7">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="8" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>0.88</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="13:18">
       <c r="M8">
         <v>3</v>
       </c>
       <c r="N8">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="9" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9" spans="13:18">
       <c r="M9">
         <v>4</v>
       </c>
       <c r="N9">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="10" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0.75</v>
+      </c>
+      <c r="Q9">
+        <v>0.95</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="13:18">
       <c r="M10">
         <v>5</v>
       </c>
       <c r="N10">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="11" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="13:18">
       <c r="M11">
         <v>6</v>
       </c>
       <c r="N11">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="12" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>0.99</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="13:18">
       <c r="M12">
         <v>7</v>
       </c>
       <c r="N12">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="13" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0.85</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="13:18">
       <c r="M13">
         <v>8</v>
       </c>
       <c r="N13">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="14" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="13:18">
       <c r="M14">
         <v>9</v>
       </c>
       <c r="N14">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="15" spans="13:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="13:18">
       <c r="M15">
         <v>10</v>
       </c>
       <c r="N15">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="16" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0.95</v>
+      </c>
+      <c r="P15">
+        <v>0.85</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="16" spans="13:18">
       <c r="N16">
         <f>AVERAGE(N6:N15)</f>
-        <v>0.9860000000000001</v>
+        <v>0.99</v>
+      </c>
+      <c r="O16">
+        <f>AVERAGE(O6:O15)</f>
+        <v>0.97999999999999987</v>
+      </c>
+      <c r="P16">
+        <f>AVERAGE(P6:P15)</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="Q16">
+        <f>AVERAGE(Q6:Q15)</f>
+        <v>0.99499999999999988</v>
+      </c>
+      <c r="R16">
+        <f>AVERAGE(R6:R15)</f>
+        <v>0.96500000000000008</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added results for training set
</commit_message>
<xml_diff>
--- a/Final Documentation/results.xlsx
+++ b/Final Documentation/results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="8250" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId5"/>
+    <sheet name="Arkusz1" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
   <si>
     <t>4 stany</t>
   </si>
@@ -44,8 +45,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +88,27 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:style val="3"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -112,6 +127,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -119,17 +135,20 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>4 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$L$3:$L$12</c:f>
@@ -176,6 +195,7 @@
           <c:tx>
             <c:v>6 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$M$3:$M$12</c:f>
@@ -222,6 +242,7 @@
           <c:tx>
             <c:v>10 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$N$3:$N$12</c:f>
@@ -268,6 +289,7 @@
           <c:tx>
             <c:v>15 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$O$3:$O$12</c:f>
@@ -308,14 +330,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="74787456"/>
-        <c:axId val="74810496"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="110879488"/>
+        <c:axId val="110881408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74787456"/>
+        <c:axId val="110879488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -334,6 +366,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -342,19 +375,23 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74810496"/>
+        <c:crossAx val="110881408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74810496"/>
+        <c:axId val="110881408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -374,6 +411,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -382,8 +420,10 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74787456"/>
+        <c:crossAx val="110879488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -400,9 +440,11 @@
           <c:h val="0.25737299107347411"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -414,8 +456,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:style val="3"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -439,18 +490,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>4 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet5!$L$4:$L$13</c:f>
@@ -497,6 +552,7 @@
           <c:tx>
             <c:v>6 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet5!$M$4:$M$13</c:f>
@@ -543,6 +599,7 @@
           <c:tx>
             <c:v>8 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet5!$N$4:$N$13</c:f>
@@ -589,6 +646,7 @@
           <c:tx>
             <c:v>10 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet5!$O$4:$O$13</c:f>
@@ -635,6 +693,7 @@
           <c:tx>
             <c:v>12 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet5!$P$4:$P$13</c:f>
@@ -675,14 +734,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="89225472"/>
-        <c:axId val="89605248"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="111856256"/>
+        <c:axId val="111866624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89225472"/>
+        <c:axId val="111856256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -701,20 +770,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89605248"/>
+        <c:crossAx val="111866624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89605248"/>
+        <c:axId val="111866624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -734,10 +808,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89225472"/>
+        <c:crossAx val="111856256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -745,8 +822,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -758,8 +838,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:style val="3"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -783,18 +872,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>4 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet6!$N$4:$N$13</c:f>
@@ -841,6 +934,7 @@
           <c:tx>
             <c:v>6 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet6!$O$4:$O$13</c:f>
@@ -887,6 +981,7 @@
           <c:tx>
             <c:v>8 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet6!$P$4:$P$13</c:f>
@@ -933,6 +1028,7 @@
           <c:tx>
             <c:v>10 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet6!$Q$4:$Q$13</c:f>
@@ -979,6 +1075,7 @@
           <c:tx>
             <c:v>12 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet6!$R$4:$R$13</c:f>
@@ -1019,14 +1116,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="102951168"/>
-        <c:axId val="102957440"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="112218880"/>
+        <c:axId val="112220800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102951168"/>
+        <c:axId val="112218880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1045,20 +1152,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102957440"/>
+        <c:crossAx val="112220800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102957440"/>
+        <c:axId val="112220800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1078,10 +1190,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102951168"/>
+        <c:crossAx val="112218880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1089,8 +1204,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1102,8 +1220,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:style val="3"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1135,18 +1262,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>4 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet7!$M$4:$M$13</c:f>
@@ -1193,6 +1324,7 @@
           <c:tx>
             <c:v>6 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet7!$N$4:$N$13</c:f>
@@ -1239,6 +1371,7 @@
           <c:tx>
             <c:v>8 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet7!$O$4:$O$13</c:f>
@@ -1285,6 +1418,7 @@
           <c:tx>
             <c:v>10 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet7!$P$4:$P$13</c:f>
@@ -1331,6 +1465,7 @@
           <c:tx>
             <c:v>12 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet7!$Q$4:$Q$13</c:f>
@@ -1371,14 +1506,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="89946368"/>
-        <c:axId val="100462592"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="112261760"/>
+        <c:axId val="112263936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89946368"/>
+        <c:axId val="112261760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1397,21 +1542,26 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100462592"/>
+        <c:crossAx val="112263936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100462592"/>
+        <c:axId val="112263936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1431,10 +1581,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89946368"/>
+        <c:crossAx val="112261760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1442,8 +1595,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1455,8 +1611,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
-  <c:style val="3"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1480,18 +1645,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>4 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet8!$N$6:$N$15</c:f>
@@ -1538,6 +1707,7 @@
           <c:tx>
             <c:v>6 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet8!$O$6:$O$15</c:f>
@@ -1584,6 +1754,7 @@
           <c:tx>
             <c:v>8 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet8!$P$6:$P$15</c:f>
@@ -1630,6 +1801,7 @@
           <c:tx>
             <c:v>10 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet8!$Q$6:$Q$15</c:f>
@@ -1676,6 +1848,7 @@
           <c:tx>
             <c:v>12 states</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet8!$R$6:$R$15</c:f>
@@ -1716,14 +1889,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60832000"/>
-        <c:axId val="61018112"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="112019712"/>
+        <c:axId val="112025984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60832000"/>
+        <c:axId val="112019712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1742,20 +1925,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61018112"/>
+        <c:crossAx val="112025984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61018112"/>
+        <c:axId val="112025984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1775,10 +1963,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60832000"/>
+        <c:crossAx val="112019712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1786,12 +1977,283 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Automata approximation - results for training set</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$L$3:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$N$3:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>15 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$O$3:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="82861440"/>
+        <c:axId val="112629248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="82861440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112629248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="112629248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82861440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86340640809443503"/>
+          <c:y val="0.42627401646544133"/>
+          <c:w val="0.1197301854974705"/>
+          <c:h val="0.25737299107347411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1974,6 +2436,43 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
@@ -2049,6 +2548,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2083,6 +2583,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2258,16 +2759,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K2:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="11:15">
+    <row r="2" spans="11:15" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
         <v>0</v>
       </c>
@@ -2281,7 +2782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="11:15">
+    <row r="3" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K3">
         <v>1</v>
       </c>
@@ -2298,7 +2799,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="11:15">
+    <row r="4" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K4">
         <v>2</v>
       </c>
@@ -2315,7 +2816,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="5" spans="11:15">
+    <row r="5" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K5">
         <v>3</v>
       </c>
@@ -2332,7 +2833,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="6" spans="11:15">
+    <row r="6" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K6">
         <v>4</v>
       </c>
@@ -2349,7 +2850,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="7" spans="11:15">
+    <row r="7" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K7">
         <v>5</v>
       </c>
@@ -2366,7 +2867,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="11:15">
+    <row r="8" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K8">
         <v>6</v>
       </c>
@@ -2383,7 +2884,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="11:15">
+    <row r="9" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K9">
         <v>7</v>
       </c>
@@ -2400,7 +2901,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="10" spans="11:15">
+    <row r="10" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K10">
         <v>8</v>
       </c>
@@ -2417,7 +2918,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="11:15">
+    <row r="11" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K11">
         <v>9</v>
       </c>
@@ -2434,7 +2935,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="12" spans="11:15">
+    <row r="12" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K12">
         <v>10</v>
       </c>
@@ -2451,7 +2952,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="11:15">
+    <row r="13" spans="11:15" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
         <v>4</v>
       </c>
@@ -2480,19 +2981,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K3:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="11:16">
+    <row r="3" spans="11:16" x14ac:dyDescent="0.25">
       <c r="L3" t="s">
         <v>0</v>
       </c>
@@ -2509,7 +3010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="11:16">
+    <row r="4" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K4">
         <v>1</v>
       </c>
@@ -2529,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="11:16">
+    <row r="5" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K5">
         <v>2</v>
       </c>
@@ -2549,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="11:16">
+    <row r="6" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K6">
         <v>3</v>
       </c>
@@ -2569,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="11:16">
+    <row r="7" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K7">
         <v>4</v>
       </c>
@@ -2589,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="11:16">
+    <row r="8" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K8">
         <v>5</v>
       </c>
@@ -2609,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="11:16">
+    <row r="9" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K9">
         <v>6</v>
       </c>
@@ -2629,7 +3130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="11:16">
+    <row r="10" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K10">
         <v>7</v>
       </c>
@@ -2649,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="11:16">
+    <row r="11" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K11">
         <v>8</v>
       </c>
@@ -2669,7 +3170,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="12" spans="11:16">
+    <row r="12" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K12">
         <v>9</v>
       </c>
@@ -2689,7 +3190,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="13" spans="11:16">
+    <row r="13" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K13">
         <v>10</v>
       </c>
@@ -2709,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="11:16">
+    <row r="14" spans="11:16" x14ac:dyDescent="0.25">
       <c r="L14">
         <f>AVERAGE(L4:L13)</f>
         <v>0.95100000000000018</v>
@@ -2739,16 +3240,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="M3:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="13:18">
+    <row r="3" spans="13:18" x14ac:dyDescent="0.25">
       <c r="N3" t="s">
         <v>0</v>
       </c>
@@ -2765,7 +3266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="13:18">
+    <row r="4" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M4">
         <v>1</v>
       </c>
@@ -2785,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="13:18">
+    <row r="5" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M5">
         <v>2</v>
       </c>
@@ -2805,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="13:18">
+    <row r="6" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M6">
         <v>3</v>
       </c>
@@ -2825,7 +3326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="13:18">
+    <row r="7" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M7">
         <v>4</v>
       </c>
@@ -2845,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="13:18">
+    <row r="8" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M8">
         <v>5</v>
       </c>
@@ -2865,7 +3366,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="9" spans="13:18">
+    <row r="9" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M9">
         <v>6</v>
       </c>
@@ -2885,7 +3386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="13:18">
+    <row r="10" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M10">
         <v>7</v>
       </c>
@@ -2905,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="13:18">
+    <row r="11" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M11">
         <v>8</v>
       </c>
@@ -2925,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="13:18">
+    <row r="12" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M12">
         <v>9</v>
       </c>
@@ -2945,7 +3446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="13:18">
+    <row r="13" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M13">
         <v>10</v>
       </c>
@@ -2965,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="13:18">
+    <row r="14" spans="13:18" x14ac:dyDescent="0.25">
       <c r="N14">
         <f>AVERAGE(N4:N13)</f>
         <v>0.94100000000000006</v>
@@ -2995,16 +3496,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L3:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="12:17">
+    <row r="3" spans="12:17" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
         <v>0</v>
       </c>
@@ -3021,7 +3522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="12:17">
+    <row r="4" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L4">
         <v>1</v>
       </c>
@@ -3041,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="12:17">
+    <row r="5" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L5">
         <v>2</v>
       </c>
@@ -3061,7 +3562,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="12:17">
+    <row r="6" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L6">
         <v>3</v>
       </c>
@@ -3081,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="12:17">
+    <row r="7" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L7">
         <v>4</v>
       </c>
@@ -3101,7 +3602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="12:17">
+    <row r="8" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L8">
         <v>5</v>
       </c>
@@ -3121,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="12:17">
+    <row r="9" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L9">
         <v>6</v>
       </c>
@@ -3141,7 +3642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="12:17">
+    <row r="10" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L10">
         <v>7</v>
       </c>
@@ -3161,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="12:17">
+    <row r="11" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L11">
         <v>8</v>
       </c>
@@ -3181,7 +3682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="12:17">
+    <row r="12" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L12">
         <v>9</v>
       </c>
@@ -3201,7 +3702,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="13" spans="12:17">
+    <row r="13" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L13">
         <v>10</v>
       </c>
@@ -3221,7 +3722,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="12:17">
+    <row r="14" spans="12:17" x14ac:dyDescent="0.25">
       <c r="M14">
         <f>AVERAGE(M4:M13)</f>
         <v>0.96799999999999997</v>
@@ -3251,16 +3752,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="M5:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="13:18">
+    <row r="5" spans="13:18" x14ac:dyDescent="0.25">
       <c r="N5" t="s">
         <v>0</v>
       </c>
@@ -3277,7 +3778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="13:18">
+    <row r="6" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M6">
         <v>1</v>
       </c>
@@ -3297,7 +3798,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="13:18">
+    <row r="7" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M7">
         <v>2</v>
       </c>
@@ -3317,7 +3818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="13:18">
+    <row r="8" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M8">
         <v>3</v>
       </c>
@@ -3337,7 +3838,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="9" spans="13:18">
+    <row r="9" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M9">
         <v>4</v>
       </c>
@@ -3357,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="13:18">
+    <row r="10" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M10">
         <v>5</v>
       </c>
@@ -3377,7 +3878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="13:18">
+    <row r="11" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M11">
         <v>6</v>
       </c>
@@ -3397,7 +3898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="13:18">
+    <row r="12" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M12">
         <v>7</v>
       </c>
@@ -3417,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="13:18">
+    <row r="13" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M13">
         <v>8</v>
       </c>
@@ -3437,7 +3938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="13:18">
+    <row r="14" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M14">
         <v>9</v>
       </c>
@@ -3457,7 +3958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="13:18">
+    <row r="15" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M15">
         <v>10</v>
       </c>
@@ -3477,7 +3978,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="16" spans="13:18">
+    <row r="16" spans="13:18" x14ac:dyDescent="0.25">
       <c r="N16">
         <f>AVERAGE(N6:N15)</f>
         <v>0.99</v>
@@ -3504,4 +4005,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="K2:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="6" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="7" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="8" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="9" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="10" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="11" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="12" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="13" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <f>AVERAGE(L3:L12)</f>
+        <v>0.41900000000000004</v>
+      </c>
+      <c r="M13" t="e">
+        <f t="shared" ref="M13:O13" si="0">AVERAGE(M3:M12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
results for training set
</commit_message>
<xml_diff>
--- a/Final Documentation/results.xlsx
+++ b/Final Documentation/results.xlsx
@@ -13,13 +13,17 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId5"/>
     <sheet name="Arkusz1" sheetId="9" r:id="rId6"/>
+    <sheet name="Arkusz2" sheetId="10" r:id="rId7"/>
+    <sheet name="Arkusz3" sheetId="11" r:id="rId8"/>
+    <sheet name="Arkusz4" sheetId="12" r:id="rId9"/>
+    <sheet name="Arkusz5" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="7">
   <si>
     <t>4 stany</t>
   </si>
@@ -80,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -339,11 +344,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="110879488"/>
-        <c:axId val="110881408"/>
+        <c:axId val="108004480"/>
+        <c:axId val="108006400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110879488"/>
+        <c:axId val="108004480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110881408"/>
+        <c:crossAx val="108006400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -386,7 +391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110881408"/>
+        <c:axId val="108006400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -423,7 +428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110879488"/>
+        <c:crossAx val="108004480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -449,6 +454,388 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>80 states</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz5!$N$6:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz5!$O$6:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz5!$P$6:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz5!$Q$6:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz5!$R$6:$R$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="51357568"/>
+        <c:axId val="51359744"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="51357568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51359744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51359744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51357568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -743,11 +1130,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="111856256"/>
-        <c:axId val="111866624"/>
+        <c:axId val="108399616"/>
+        <c:axId val="108409984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111856256"/>
+        <c:axId val="108399616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +1162,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111866624"/>
+        <c:crossAx val="108409984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -783,7 +1170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111866624"/>
+        <c:axId val="108409984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -814,7 +1201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111856256"/>
+        <c:crossAx val="108399616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1125,11 +1512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="112218880"/>
-        <c:axId val="112220800"/>
+        <c:axId val="108164224"/>
+        <c:axId val="108166144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112218880"/>
+        <c:axId val="108164224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1157,7 +1544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112220800"/>
+        <c:crossAx val="108166144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1165,7 +1552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112220800"/>
+        <c:axId val="108166144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1196,7 +1583,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112218880"/>
+        <c:crossAx val="108164224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1515,11 +1902,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="112261760"/>
-        <c:axId val="112263936"/>
+        <c:axId val="108272640"/>
+        <c:axId val="108278912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112261760"/>
+        <c:axId val="108272640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,7 +1934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112263936"/>
+        <c:crossAx val="108278912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1555,7 +1942,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112263936"/>
+        <c:axId val="108278912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1587,7 +1974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112261760"/>
+        <c:crossAx val="108272640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1898,11 +2285,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="112019712"/>
-        <c:axId val="112025984"/>
+        <c:axId val="108751104"/>
+        <c:axId val="108761472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112019712"/>
+        <c:axId val="108751104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1930,7 +2317,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112025984"/>
+        <c:crossAx val="108761472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1938,7 +2325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112025984"/>
+        <c:axId val="108761472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1969,7 +2356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112019712"/>
+        <c:crossAx val="108751104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2048,37 +2435,37 @@
             <c:numRef>
               <c:f>Arkusz1!$L$3:$L$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.54</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.37</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.48</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2095,8 +2482,38 @@
             <c:numRef>
               <c:f>Arkusz1!$M$3:$M$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.08</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2112,8 +2529,38 @@
             <c:numRef>
               <c:f>Arkusz1!$N$3:$N$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2129,8 +2576,38 @@
             <c:numRef>
               <c:f>Arkusz1!$O$3:$O$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2144,11 +2621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82861440"/>
-        <c:axId val="112629248"/>
+        <c:axId val="108809600"/>
+        <c:axId val="108824064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82861440"/>
+        <c:axId val="108809600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2183,7 +2660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112629248"/>
+        <c:crossAx val="108824064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2191,7 +2668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112629248"/>
+        <c:axId val="108824064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2224,11 +2701,11 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82861440"/>
+        <c:crossAx val="108809600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2259,6 +2736,1161 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>20 states</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$L$4:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$M$4:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="53248000"/>
+        <c:axId val="53249920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="53248000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53249920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="53249920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53248000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>30 states</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz3!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz3!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz3!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz3!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz3!$R$4:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="79897728"/>
+        <c:axId val="79899648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="79897728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79899648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79899648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79897728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>50</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>states</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> automaton approximation</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz4!$M$4:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>6 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz4!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>8 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz4!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz4!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>12 states</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz4!$Q$4:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="80471168"/>
+        <c:axId val="80473088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="80471168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Iteration number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80473088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80473088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Error rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80471168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2277,6 +3909,43 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1025" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2454,6 +4123,117 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="9" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2762,7 +4542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K2:O13"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -2975,6 +4755,261 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="M5:R16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0.99</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0.99</v>
+      </c>
+      <c r="Q6">
+        <v>0.86</v>
+      </c>
+      <c r="R6">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0.97</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0.98</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0.98</v>
+      </c>
+      <c r="R8">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="9" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>0.96</v>
+      </c>
+      <c r="O9">
+        <v>0.99</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0.99</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0.99</v>
+      </c>
+      <c r="P10">
+        <v>0.98</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="11" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>0.92</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0.97</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>7</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0.99</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="13" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>8</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0.94</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0.99</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>9</v>
+      </c>
+      <c r="N14">
+        <v>0.99</v>
+      </c>
+      <c r="O14">
+        <v>0.97</v>
+      </c>
+      <c r="P14">
+        <v>0.96</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="15" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>0.98</v>
+      </c>
+      <c r="O15">
+        <v>0.99</v>
+      </c>
+      <c r="P15">
+        <v>0.99</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <f>AVERAGE(N6:N15)</f>
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="O16">
+        <f>AVERAGE(O6:O15)</f>
+        <v>0.9860000000000001</v>
+      </c>
+      <c r="P16">
+        <f>AVERAGE(P6:P15)</f>
+        <v>0.9880000000000001</v>
+      </c>
+      <c r="Q16">
+        <f>AVERAGE(Q6:Q15)</f>
+        <v>0.97899999999999987</v>
+      </c>
+      <c r="R16">
+        <f>AVERAGE(R6:R15)</f>
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2985,7 +5020,7 @@
   <dimension ref="K3:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,7 +5279,7 @@
   <dimension ref="M3:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3500,7 +5535,7 @@
   <dimension ref="L3:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3756,7 +5791,7 @@
   <dimension ref="M5:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD1048576"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,124 +6047,986 @@
   <dimension ref="K2:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="V13" sqref="V13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="15" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M3" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="7" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="8" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="11" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="12" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="13" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1">
+        <f>AVERAGE(L3:L12)</f>
+        <v>0.23800000000000004</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" ref="M13:O13" si="0">AVERAGE(M3:M12)</f>
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="K3:P14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0.89</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0.93</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>0.99</v>
+      </c>
+      <c r="M5">
+        <v>0.91</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0.81</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0.83</v>
+      </c>
+      <c r="N6">
+        <v>0.98</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>0.86</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0.62</v>
+      </c>
+      <c r="O7">
+        <v>0.96</v>
+      </c>
+      <c r="P7">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="8" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0.98</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0.85</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0.97</v>
+      </c>
+      <c r="N9">
+        <v>0.99</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="10" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <v>0.97</v>
+      </c>
+      <c r="M10">
+        <v>0.98</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0.98</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <v>0.85</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0.97</v>
+      </c>
+      <c r="O11">
+        <v>0.96</v>
+      </c>
+      <c r="P11">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>9</v>
+      </c>
+      <c r="L12">
+        <v>0.93</v>
+      </c>
+      <c r="M12">
+        <v>0.81</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="13" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0.98</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f>AVERAGE(L4:L13)</f>
+        <v>0.94900000000000007</v>
+      </c>
+      <c r="M14">
+        <f>AVERAGE(M4:M13)</f>
+        <v>0.94800000000000006</v>
+      </c>
+      <c r="N14">
+        <f>AVERAGE(N4:N13)</f>
+        <v>0.94700000000000006</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(O4:O13)</f>
+        <v>0.95599999999999985</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(P4:P13)</f>
+        <v>0.96200000000000008</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="M3:R14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="L2" t="s">
+    <row r="3" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
         <v>2</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0.73</v>
+      </c>
+      <c r="P4">
+        <v>0.99</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="5" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>0.98</v>
+      </c>
+      <c r="O5">
+        <v>0.98</v>
+      </c>
+      <c r="P5">
+        <v>0.88</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="6" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M6">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K4">
+      <c r="N6">
+        <v>0.93</v>
+      </c>
+      <c r="O6">
+        <v>0.99</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0.98</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>0.75</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0.93</v>
+      </c>
+      <c r="R7">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="8" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0.94</v>
+      </c>
+      <c r="P8">
+        <v>0.78</v>
+      </c>
+      <c r="Q8">
+        <v>0.82</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0.96</v>
+      </c>
+      <c r="P9">
+        <v>0.99</v>
+      </c>
+      <c r="Q9">
+        <v>0.99</v>
+      </c>
+      <c r="R9">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="10" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>7</v>
+      </c>
+      <c r="N10">
+        <v>0.99</v>
+      </c>
+      <c r="O10">
+        <v>0.99</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0.98</v>
+      </c>
+      <c r="R10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>8</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0.98</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>9</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0.99</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="N13">
+        <v>0.96</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0.98</v>
+      </c>
+      <c r="R13">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="14" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <f>AVERAGE(N4:N13)</f>
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(O4:O13)</f>
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(P4:P13)</f>
+        <v>0.96200000000000008</v>
+      </c>
+      <c r="Q14">
+        <f>AVERAGE(Q4:Q13)</f>
+        <v>0.96800000000000019</v>
+      </c>
+      <c r="R14">
+        <f>AVERAGE(R4:R13)</f>
+        <v>0.96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="L3:Q14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" t="s">
         <v>2</v>
       </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="12:17" x14ac:dyDescent="0.25">
       <c r="L4">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0.99</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0.85</v>
+      </c>
+      <c r="Q4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0.98</v>
+      </c>
+      <c r="N5">
+        <v>0.88</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L6">
         <v>3</v>
       </c>
-      <c r="L5">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="6" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K6">
+      <c r="M6">
+        <v>0.99</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0.98</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="7" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L7">
         <v>4</v>
       </c>
-      <c r="L6">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="7" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K7">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0.87</v>
+      </c>
+      <c r="P7">
+        <v>0.97</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L8">
         <v>5</v>
       </c>
-      <c r="L7">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="8" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K8">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0.92</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0.99</v>
+      </c>
+      <c r="Q8">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="9" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L9">
         <v>6</v>
       </c>
-      <c r="L8">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="9" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K9">
+      <c r="M9">
+        <v>0.86</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0.92</v>
+      </c>
+      <c r="P9">
+        <v>0.89</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L10">
         <v>7</v>
       </c>
-      <c r="L9">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="10" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K10">
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0.89</v>
+      </c>
+      <c r="O10">
+        <v>0.97</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L11">
         <v>8</v>
       </c>
-      <c r="L10">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="11" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K11">
+      <c r="M11">
+        <v>0.98</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L12">
         <v>9</v>
       </c>
-      <c r="L11">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="12" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K12">
+      <c r="M12">
+        <v>0.89</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0.99</v>
+      </c>
+      <c r="P12">
+        <v>0.99</v>
+      </c>
+      <c r="Q12">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="13" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L13">
         <v>10</v>
       </c>
-      <c r="L12">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="13" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K13" t="s">
-        <v>4</v>
-      </c>
-      <c r="L13">
-        <f>AVERAGE(L3:L12)</f>
-        <v>0.41900000000000004</v>
-      </c>
-      <c r="M13" t="e">
-        <f t="shared" ref="M13:O13" si="0">AVERAGE(M3:M12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0.98</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f>AVERAGE(M4:M13)</f>
+        <v>0.97000000000000008</v>
+      </c>
+      <c r="N14">
+        <f>AVERAGE(N4:N13)</f>
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(O4:O13)</f>
+        <v>0.97099999999999986</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(P4:P13)</f>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="Q14">
+        <f>AVERAGE(Q4:Q13)</f>
+        <v>0.97399999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>